<commit_message>
Update scripts and documentation, exclude large simg files
</commit_message>
<xml_diff>
--- a/Other_tools/5_sra数据提交/ngdc/Plant.cn.xlsx
+++ b/Other_tools/5_sra数据提交/ngdc/Plant.cn.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="10480"/>
+    <workbookView windowWidth="24750" windowHeight="12080"/>
   </bookViews>
   <sheets>
     <sheet name="Plant" sheetId="2" r:id="rId1"/>
@@ -486,7 +486,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="489" uniqueCount="123">
   <si>
     <r>
       <rPr>
@@ -1290,7 +1290,7 @@
     <t>treatment</t>
   </si>
   <si>
-    <t>Calathodes_oxycarpa_2024050902-8</t>
+    <t>rna-Calathodes_oxycarpa_2024050902-8</t>
   </si>
   <si>
     <r>
@@ -1332,7 +1332,7 @@
     <t>year</t>
   </si>
   <si>
-    <t>Trollius_altaicus20240618009</t>
+    <t>rna-Trollius_altaicus20240618009</t>
   </si>
   <si>
     <r>
@@ -1359,7 +1359,7 @@
     <t>Trollius altaicus</t>
   </si>
   <si>
-    <t>Trollius_chinensis2023061310</t>
+    <t>rna-Trollius_chinensis2023061310</t>
   </si>
   <si>
     <r>
@@ -1386,7 +1386,7 @@
     <t>Trollius chinensis</t>
   </si>
   <si>
-    <t>Trollius_lilacinus20240611005</t>
+    <t>rna-Trollius_lilacinus20240611005</t>
   </si>
   <si>
     <r>
@@ -1413,7 +1413,7 @@
     <t>Trollius lilacinus</t>
   </si>
   <si>
-    <t>Trollius_pumilus2023080915</t>
+    <t>rna-Trollius_pumilus2023080915</t>
   </si>
   <si>
     <r>
@@ -1440,7 +1440,7 @@
     <t>Trollius pumilus</t>
   </si>
   <si>
-    <t>Trollius_ranunculoides2024060502</t>
+    <t>rna-Trollius_ranunculoides2024060502</t>
   </si>
   <si>
     <r>
@@ -1467,7 +1467,7 @@
     <t>Trollius ranunculoides</t>
   </si>
   <si>
-    <t>Trollius_yunnanensis2023081015-1</t>
+    <t>rna-Trollius_yunnanensis2023081015-1</t>
   </si>
   <si>
     <r>
@@ -1494,7 +1494,7 @@
     <t>Trollius yunnanensis</t>
   </si>
   <si>
-    <t>Adonis_aestivalis_var_parviflora_I-4422</t>
+    <t>rna-Adonis_aestivalis_var_parviflora_I-4422</t>
   </si>
   <si>
     <r>
@@ -1540,7 +1540,7 @@
     <t>Adonis aestivalis</t>
   </si>
   <si>
-    <t>Adonis_amurensis_ChengnanPark2025031401</t>
+    <t>rna-Adonis_amurensis_ChengnanPark2025031401</t>
   </si>
   <si>
     <r>
@@ -1567,19 +1567,19 @@
     <t>Adonis amurensis</t>
   </si>
   <si>
-    <t>Adonis_amurensis_Japan_WHJP01</t>
-  </si>
-  <si>
-    <t>Adonis_amurensis_Tonghua_1_2024050405-1</t>
-  </si>
-  <si>
-    <t>Adonis_amurensis_Tonghua_2024050305-1</t>
-  </si>
-  <si>
-    <t>Adonis_amurensis_Tonghua_3_2024050405-3</t>
-  </si>
-  <si>
-    <t>Adonis_bobroviana_1_2024060601-1</t>
+    <t>rna-Adonis_amurensis_Japan_WHJP01</t>
+  </si>
+  <si>
+    <t>rna-Adonis_amurensis_Tonghua_1_2024050405-1</t>
+  </si>
+  <si>
+    <t>rna-Adonis_amurensis_Tonghua_2024050305-1</t>
+  </si>
+  <si>
+    <t>rna-Adonis_amurensis_Tonghua_3_2024050405-3</t>
+  </si>
+  <si>
+    <t>rna-Adonis_bobroviana_1_2024060601-1</t>
   </si>
   <si>
     <r>
@@ -1606,13 +1606,13 @@
     <t>Adonis bobroviana</t>
   </si>
   <si>
-    <t>Adonis_bobroviana_2_2024060601-2</t>
-  </si>
-  <si>
-    <t>Adonis_bobroviana_3_2024060601-3</t>
-  </si>
-  <si>
-    <t>Adonis_coerulea_1_2024060508-1</t>
+    <t>rna-Adonis_bobroviana_2_2024060601-2</t>
+  </si>
+  <si>
+    <t>rna-Adonis_bobroviana_3_2024060601-3</t>
+  </si>
+  <si>
+    <t>rna-Adonis_coerulea_1_2024060508-1</t>
   </si>
   <si>
     <r>
@@ -1639,13 +1639,13 @@
     <t>Adonis coerulea</t>
   </si>
   <si>
-    <t>Adonis_coerulea_2_2024060508-2</t>
-  </si>
-  <si>
-    <t>Adonis_coerulea_3_2024060508-3</t>
-  </si>
-  <si>
-    <t>Adonis_davidii_2025050306-12</t>
+    <t>rna-Adonis_coerulea_2_2024060508-2</t>
+  </si>
+  <si>
+    <t>rna-Adonis_coerulea_3_2024060508-3</t>
+  </si>
+  <si>
+    <t>rna-Adonis_davidii_2025050306-12</t>
   </si>
   <si>
     <r>
@@ -1672,13 +1672,13 @@
     <t>Adonis brevistyla</t>
   </si>
   <si>
-    <t>Adonis_davidii_2025050306-1</t>
-  </si>
-  <si>
-    <t>Adonis_davidii_2025050306-9</t>
-  </si>
-  <si>
-    <t>Adonis_fupingensis2_2023051702</t>
+    <t>rna-Adonis_davidii_2025050306-1</t>
+  </si>
+  <si>
+    <t>rna-Adonis_davidii_2025050306-9</t>
+  </si>
+  <si>
+    <t>rna-Adonis_fupingensis2_2023051702</t>
   </si>
   <si>
     <r>
@@ -1705,191 +1705,176 @@
     <t>Adonis ramosa</t>
   </si>
   <si>
-    <t>Adonis_fupingensis4_2023051704</t>
-  </si>
-  <si>
-    <t>Adonis_fupingensis5_2023051705</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_chashikou2024030801</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">RNA-SEQ of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+    <t>rna-Adonis_fupingensis4_2023051704</t>
+  </si>
+  <si>
+    <t>rna-Adonis_fupingensis5_2023051705</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_chashikou2024030801</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t>Adonis ramosa</t>
-    </r>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Henan-4_2025031201-4</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
+      <t xml:space="preserve">RNA-SEQ of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">RNA-SEQ of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+      <t>Adonis ramosa</t>
+    </r>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Henan-4_2025031201-4</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Henan_17_2025031201-17</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Henan_5_2025031201-5</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Huairou_Fenghuangtuo_2025032802-3</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Jiangsu_01_2025032301-1</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Jiangsu_03_2025032303-1</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Shandong-9_2025041001-9</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Shandong_1_2025041001-1</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Shandong_5_2025041001-5</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Tonghua_1_2024050304-1</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Tonghua_2024050304-2</t>
+  </si>
+  <si>
+    <t>rna-Adonis_ramosa_Tonghua_5_2024050304-5</t>
+  </si>
+  <si>
+    <t>rna-Adonis_sibirica_20250527001</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t>Adonis ramosa</t>
-    </r>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Henan_17_2025031201-17</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Henan_5_2025031201-5</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Huairou_Fenghuangtuo_2025032802-3</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Jiangsu_01_2025032301-1</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Jiangsu_03_2025032303-1</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Shandong-9_2025041001-9</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Shandong_1_2025041001-1</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Shandong_5_2025041001-5</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Tonghua_1_2024050304-1</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Tonghua_2024050304-2</t>
-  </si>
-  <si>
-    <t>Adonis_ramosa_Tonghua_5_2024050304-5</t>
-  </si>
-  <si>
-    <t>Adonis_sibirica_20250527001</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
+      <t xml:space="preserve">RNA-SEQ of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">RNA-SEQ of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+      <t>Adonis sibirica</t>
+    </r>
+  </si>
+  <si>
+    <t>Adonis sibirica</t>
+  </si>
+  <si>
+    <t>rna-Adonis_sibirica_4786_I-4786</t>
+  </si>
+  <si>
+    <t>rna-Adonis_sibirica_I-4749_I-4749</t>
+  </si>
+  <si>
+    <t>rna-Adonis_sutchuenensis_1_WH25032502</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t>Adonis sibirica</t>
-    </r>
-  </si>
-  <si>
-    <t>Adonis sibirica</t>
-  </si>
-  <si>
-    <t>Adonis_sibirica_4786_I-4786</t>
-  </si>
-  <si>
-    <t>Adonis_sibirica_I-4749_I-4749</t>
-  </si>
-  <si>
-    <t>Adonis_sutchuenensis_1_WH25032502</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
+      <t xml:space="preserve">RNA-SEQ of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">RNA-SEQ of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+      <t>Adonis sutchuenensis</t>
+    </r>
+  </si>
+  <si>
+    <t>Adonis sutchuenensis</t>
+  </si>
+  <si>
+    <t>rna-Adonis_sutchuenensis_2_WH25032502-2</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t>Adonis sutchuenensis</t>
-    </r>
-  </si>
-  <si>
-    <t>Adonis sutchuenensis</t>
-  </si>
-  <si>
-    <t>Adonis_sutchuenensis_2_WH25032502-2</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
+      <t>RNA-SEQ of</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t>RNA-SEQ of</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
+      <t xml:space="preserve"> Adonis sutchuenensis</t>
+    </r>
+  </si>
+  <si>
+    <t>rna-Adonis_villosa_4247_I-4247</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve"> Adonis sutchuenensis</t>
-    </r>
-  </si>
-  <si>
-    <t>Adonis_villosa_4247_I-4247</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
+      <t xml:space="preserve">RNA-SEQ of </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
         <sz val="11"/>
         <color theme="1"/>
         <rFont val="Times New Roman"/>
         <charset val="134"/>
       </rPr>
-      <t xml:space="preserve">RNA-SEQ of </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <charset val="134"/>
-      </rPr>
       <t>Adonis villosa</t>
     </r>
   </si>
@@ -1897,7 +1882,7 @@
     <t>Adonis villosa</t>
   </si>
   <si>
-    <t>Adonis_villosa_lll20240520011</t>
+    <t>rna-Adonis_villosa_lll20240520011</t>
   </si>
 </sst>
 </file>
@@ -1905,14 +1890,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="6">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="178" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="179" formatCode="yyyy/mm/dd"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2116,13 +2101,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
@@ -2144,6 +2122,13 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Adobe 黑体 Std R"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Adobe 黑体 Std R"/>
       <charset val="134"/>
@@ -2155,22 +2140,8 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <name val="Adobe 黑体 Std R"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Adobe 黑体 Std R"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Adobe 黑体 Std R"/>
+      <sz val="9"/>
+      <name val="等线"/>
       <charset val="134"/>
     </font>
     <font>
@@ -2178,14 +2149,8 @@
       <name val="等线"/>
       <charset val="134"/>
     </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <name val="等线"/>
-      <charset val="134"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2219,12 +2184,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2637,28 +2596,28 @@
   </borders>
   <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2682,16 +2641,16 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="8" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="17" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -2700,89 +2659,89 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -3271,16 +3230,16 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AD564"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.78181818181818" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="138.272727272727" style="4" customWidth="1"/>
+    <col min="1" max="1" width="63.2454545454545" style="4" customWidth="1"/>
     <col min="2" max="2" width="42.7272727272727" style="5" customWidth="1"/>
     <col min="3" max="3" width="22.1090909090909" style="4" customWidth="1"/>
-    <col min="4" max="4" width="17.6636363636364" style="4" customWidth="1"/>
+    <col min="4" max="4" width="54.0181818181818" style="4" customWidth="1"/>
     <col min="5" max="5" width="30.0909090909091" style="4" customWidth="1"/>
     <col min="6" max="6" width="12" style="4" customWidth="1"/>
     <col min="7" max="7" width="25.4454545454545" style="4" customWidth="1"/>
@@ -4579,13 +4538,13 @@
         <v>97</v>
       </c>
       <c r="B37" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D37" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E37" s="25" t="s">
         <v>92</v>
@@ -4608,16 +4567,16 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B38" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E38" s="25" t="s">
         <v>92</v>
@@ -4640,16 +4599,16 @@
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="23" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B39" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D39" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E39" s="25" t="s">
         <v>92</v>
@@ -4672,16 +4631,16 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="23" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B40" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D40" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E40" s="25" t="s">
         <v>92</v>
@@ -4704,16 +4663,16 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="23" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B41" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D41" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E41" s="25" t="s">
         <v>92</v>
@@ -4736,16 +4695,16 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D42" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E42" s="25" t="s">
         <v>92</v>
@@ -4768,16 +4727,16 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="23" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B43" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D43" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E43" s="25" t="s">
         <v>92</v>
@@ -4800,16 +4759,16 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="23" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B44" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E44" s="25" t="s">
         <v>92</v>
@@ -4832,16 +4791,16 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="23" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B45" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D45" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E45" s="25" t="s">
         <v>92</v>
@@ -4864,16 +4823,16 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="23" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B46" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D46" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E46" s="25" t="s">
         <v>92</v>
@@ -4896,16 +4855,16 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B47" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D47" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E47" s="25" t="s">
         <v>92</v>
@@ -4928,16 +4887,16 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="23" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B48" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D48" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E48" s="25" t="s">
         <v>92</v>
@@ -4960,19 +4919,19 @@
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="B49" s="24" t="s">
         <v>110</v>
-      </c>
-      <c r="B49" s="24" t="s">
-        <v>111</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D49" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E49" s="25" t="s">
         <v>111</v>
-      </c>
-      <c r="E49" s="25" t="s">
-        <v>112</v>
       </c>
       <c r="F49" s="4" t="s">
         <v>43</v>
@@ -4992,19 +4951,19 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="23" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B50" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D50" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E50" s="25" t="s">
         <v>111</v>
-      </c>
-      <c r="E50" s="25" t="s">
-        <v>112</v>
       </c>
       <c r="F50" s="4" t="s">
         <v>43</v>
@@ -5024,19 +4983,19 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="23" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B51" s="24" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C51" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D51" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="E51" s="25" t="s">
         <v>111</v>
-      </c>
-      <c r="E51" s="25" t="s">
-        <v>112</v>
       </c>
       <c r="F51" s="4" t="s">
         <v>43</v>
@@ -5056,19 +5015,19 @@
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="B52" s="24" t="s">
         <v>115</v>
-      </c>
-      <c r="B52" s="24" t="s">
-        <v>116</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D52" s="24" t="s">
+        <v>115</v>
+      </c>
+      <c r="E52" s="25" t="s">
         <v>116</v>
-      </c>
-      <c r="E52" s="25" t="s">
-        <v>117</v>
       </c>
       <c r="F52" s="4" t="s">
         <v>43</v>
@@ -5088,19 +5047,19 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="B53" s="24" t="s">
         <v>118</v>
-      </c>
-      <c r="B53" s="24" t="s">
-        <v>119</v>
       </c>
       <c r="C53" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E53" s="25" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>43</v>
@@ -5120,19 +5079,19 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="B54" s="24" t="s">
         <v>120</v>
-      </c>
-      <c r="B54" s="24" t="s">
-        <v>121</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>41</v>
       </c>
       <c r="D54" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" s="25" t="s">
         <v>121</v>
-      </c>
-      <c r="E54" s="25" t="s">
-        <v>122</v>
       </c>
       <c r="F54" s="4" t="s">
         <v>43</v>
@@ -5152,19 +5111,19 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C55" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D55" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="25" t="s">
         <v>121</v>
-      </c>
-      <c r="E55" s="25" t="s">
-        <v>122</v>
       </c>
       <c r="F55" s="4" t="s">
         <v>43</v>
@@ -7229,7 +7188,7 @@
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:J55 J56:J1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J11:J1048576">
       <formula1>"year,month,day,week,hour,minute,second"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AA11:AA1048576">

</xml_diff>